<commit_message>
Verified BOM correctness and availabity of parts
</commit_message>
<xml_diff>
--- a/Documents/BOM V2/Music_Visualizer_BOM_Digikey_Final_V2.xlsx
+++ b/Documents/BOM V2/Music_Visualizer_BOM_Digikey_Final_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\BOM V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFE2B9E-90F8-474E-92D3-27335415644A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C226EC-E192-40CC-A4B3-53C43B144991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19410" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1154,15 +1154,6 @@
     <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07390KL/727199</t>
   </si>
   <si>
-    <t>311-4012-1-ND</t>
-  </si>
-  <si>
-    <t>CC0603JRX7R9BB273</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/yageo/CC0603JRX7R9BB273/5883686</t>
-  </si>
-  <si>
     <t>490-GRM31CD80J107MEA8KCT-ND</t>
   </si>
   <si>
@@ -1329,14 +1320,24 @@
   </si>
   <si>
     <t>https://www.digikey.ca/en/products/detail/walsin-technology-corporation/0603N821J500CT/9355045</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/kyocera-avx/KAF15AR71H273JM/3660870</t>
+  </si>
+  <si>
+    <t>478-KAF15AR71H273JMTR-ND</t>
+  </si>
+  <si>
+    <t>KAF15AR71H273JM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -1820,10 +1821,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2184,7 +2186,10 @@
   <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2460,10 +2465,10 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="F9" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="G9" s="2">
         <v>0.11</v>
@@ -2473,7 +2478,7 @@
         <v>0.22</v>
       </c>
       <c r="I9" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -2491,28 +2496,28 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>373</v>
+        <v>430</v>
       </c>
       <c r="F10" t="s">
-        <v>374</v>
+        <v>431</v>
       </c>
       <c r="G10" s="2">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" si="0"/>
-        <v>0.38</v>
+        <v>0.36</v>
       </c>
       <c r="I10" t="s">
-        <v>375</v>
+        <v>429</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B11" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -2521,10 +2526,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="F11" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="G11" s="2">
         <v>0.14000000000000001</v>
@@ -2534,7 +2539,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="I11" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -2552,20 +2557,20 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="F12" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="G12" s="2">
-        <v>0.71</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" si="0"/>
-        <v>1.42</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I12" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -2583,20 +2588,20 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F13" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="G13" s="2">
-        <v>0.15</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="0"/>
-        <v>0.44999999999999996</v>
+        <v>0.42000000000000004</v>
       </c>
       <c r="I13" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -2614,20 +2619,20 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="F14" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="G14" s="2">
-        <v>0.24</v>
+        <v>0.34</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="0"/>
-        <v>1.68</v>
+        <v>2.3800000000000003</v>
       </c>
       <c r="I14" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -2645,20 +2650,20 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F15" t="s">
+        <v>380</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="0"/>
+        <v>1.06</v>
+      </c>
+      <c r="I15" t="s">
         <v>383</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0.92</v>
-      </c>
-      <c r="H15" s="2">
-        <f t="shared" si="0"/>
-        <v>1.84</v>
-      </c>
-      <c r="I15" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -2676,20 +2681,20 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="F16">
         <v>885012206074</v>
       </c>
       <c r="G16" s="2">
-        <v>0.15</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="I16" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -2707,20 +2712,20 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="F17">
         <v>860010372006</v>
       </c>
       <c r="G17" s="2">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="I17" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -2738,10 +2743,10 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="F18" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="G18" s="2">
         <v>0.1</v>
@@ -2751,7 +2756,7 @@
         <v>0.1</v>
       </c>
       <c r="I18" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -2769,20 +2774,20 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F19">
         <v>860010372001</v>
       </c>
       <c r="G19" s="2">
-        <v>0.15</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="I19" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -2800,20 +2805,20 @@
         <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="F20" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G20" s="2">
-        <v>0.15</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="0"/>
-        <v>2.25</v>
+        <v>2.1</v>
       </c>
       <c r="I20" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -2831,20 +2836,20 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F21" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="G21" s="2">
-        <v>0.56000000000000005</v>
+        <v>0.36</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="0"/>
-        <v>1.1200000000000001</v>
+        <v>0.72</v>
       </c>
       <c r="I21" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -2862,20 +2867,20 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="F22" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="G22" s="2">
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.72</v>
       </c>
       <c r="I22" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -2893,20 +2898,20 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F23" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="G23" s="2">
-        <v>1.49</v>
+        <v>1.42</v>
       </c>
       <c r="H23" s="2">
         <f t="shared" si="0"/>
-        <v>1.49</v>
+        <v>1.42</v>
       </c>
       <c r="I23" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -2924,20 +2929,20 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="F24" t="s">
         <v>49</v>
       </c>
       <c r="G24" s="2">
-        <v>0.8</v>
+        <v>0.69</v>
       </c>
       <c r="H24" s="2">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.69</v>
       </c>
       <c r="I24" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -2961,11 +2966,11 @@
         <v>205</v>
       </c>
       <c r="G25" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I25" t="s">
         <v>206</v>
@@ -2992,11 +2997,11 @@
         <v>208</v>
       </c>
       <c r="G26" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
+        <f>D26*G26</f>
+        <v>0.15</v>
       </c>
       <c r="I26" t="s">
         <v>209</v>
@@ -3023,11 +3028,11 @@
         <v>211</v>
       </c>
       <c r="G27" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I27" t="s">
         <v>212</v>
@@ -3054,11 +3059,11 @@
         <v>214</v>
       </c>
       <c r="G28" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I28" t="s">
         <v>215</v>
@@ -3085,11 +3090,11 @@
         <v>217</v>
       </c>
       <c r="G29" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H29" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I29" t="s">
         <v>218</v>
@@ -3116,11 +3121,11 @@
         <v>220</v>
       </c>
       <c r="G30" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H30" s="2">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
+        <f>D30*G30</f>
+        <v>0.15</v>
       </c>
       <c r="I30" t="s">
         <v>221</v>
@@ -3147,11 +3152,11 @@
         <v>223</v>
       </c>
       <c r="G31" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I31" t="s">
         <v>224</v>
@@ -3178,11 +3183,11 @@
         <v>226</v>
       </c>
       <c r="G32" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H32" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I32" t="s">
         <v>227</v>
@@ -3209,11 +3214,11 @@
         <v>229</v>
       </c>
       <c r="G33" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H33" s="2">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="I33" t="s">
         <v>230</v>
@@ -3240,11 +3245,11 @@
         <v>232</v>
       </c>
       <c r="G34" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H34" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I34" t="s">
         <v>233</v>
@@ -3271,11 +3276,11 @@
         <v>235</v>
       </c>
       <c r="G35" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H35" s="2">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="I35" t="s">
         <v>236</v>
@@ -3302,11 +3307,11 @@
         <v>238</v>
       </c>
       <c r="G36" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H36" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I36" t="s">
         <v>239</v>
@@ -3333,11 +3338,11 @@
         <v>241</v>
       </c>
       <c r="G37" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H37" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I37" t="s">
         <v>242</v>
@@ -3364,11 +3369,11 @@
         <v>244</v>
       </c>
       <c r="G38" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H38" s="2">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="I38" t="s">
         <v>245</v>
@@ -3395,11 +3400,11 @@
         <v>247</v>
       </c>
       <c r="G39" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I39" t="s">
         <v>248</v>
@@ -3426,11 +3431,11 @@
         <v>250</v>
       </c>
       <c r="G40" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H40" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I40" t="s">
         <v>251</v>
@@ -3457,11 +3462,11 @@
         <v>253</v>
       </c>
       <c r="G41" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H41" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I41" t="s">
         <v>254</v>
@@ -3488,11 +3493,11 @@
         <v>256</v>
       </c>
       <c r="G42" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H42" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I42" t="s">
         <v>257</v>
@@ -3519,11 +3524,11 @@
         <v>259</v>
       </c>
       <c r="G43" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H43" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I43" t="s">
         <v>260</v>
@@ -3550,11 +3555,11 @@
         <v>262</v>
       </c>
       <c r="G44" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H44" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I44" t="s">
         <v>263</v>
@@ -3581,11 +3586,11 @@
         <v>265</v>
       </c>
       <c r="G45" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H45" s="2">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="I45" t="s">
         <v>266</v>
@@ -3612,11 +3617,11 @@
         <v>268</v>
       </c>
       <c r="G46" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H46" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I46" t="s">
         <v>269</v>
@@ -3643,11 +3648,11 @@
         <v>271</v>
       </c>
       <c r="G47" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H47" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I47" t="s">
         <v>272</v>
@@ -3674,11 +3679,11 @@
         <v>274</v>
       </c>
       <c r="G48" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H48" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I48" t="s">
         <v>275</v>
@@ -3705,11 +3710,11 @@
         <v>277</v>
       </c>
       <c r="G49" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H49" s="2">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="I49" t="s">
         <v>278</v>
@@ -3736,11 +3741,11 @@
         <v>280</v>
       </c>
       <c r="G50" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H50" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I50" t="s">
         <v>281</v>
@@ -3767,11 +3772,11 @@
         <v>283</v>
       </c>
       <c r="G51" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H51" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I51" t="s">
         <v>284</v>
@@ -3798,11 +3803,11 @@
         <v>286</v>
       </c>
       <c r="G52" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H52" s="2">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="I52" t="s">
         <v>287</v>
@@ -3829,11 +3834,11 @@
         <v>289</v>
       </c>
       <c r="G53" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H53" s="2">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="I53" t="s">
         <v>290</v>
@@ -3860,11 +3865,11 @@
         <v>292</v>
       </c>
       <c r="G54" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H54" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I54" t="s">
         <v>293</v>
@@ -3891,11 +3896,11 @@
         <v>295</v>
       </c>
       <c r="G55" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H55" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I55" t="s">
         <v>296</v>
@@ -3922,11 +3927,11 @@
         <v>298</v>
       </c>
       <c r="G56" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H56" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I56" t="s">
         <v>299</v>
@@ -3953,11 +3958,11 @@
         <v>301</v>
       </c>
       <c r="G57" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H57" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I57" t="s">
         <v>302</v>
@@ -3984,11 +3989,11 @@
         <v>304</v>
       </c>
       <c r="G58" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H58" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I58" t="s">
         <v>305</v>
@@ -4015,11 +4020,11 @@
         <v>307</v>
       </c>
       <c r="G59" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H59" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I59" t="s">
         <v>308</v>
@@ -4046,11 +4051,11 @@
         <v>310</v>
       </c>
       <c r="G60" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H60" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I60" t="s">
         <v>311</v>
@@ -4077,11 +4082,11 @@
         <v>313</v>
       </c>
       <c r="G61" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H61" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I61" t="s">
         <v>314</v>
@@ -4108,11 +4113,11 @@
         <v>316</v>
       </c>
       <c r="G62" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H62" s="2">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="I62" t="s">
         <v>317</v>
@@ -4139,11 +4144,11 @@
         <v>319</v>
       </c>
       <c r="G63" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H63" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I63" t="s">
         <v>320</v>
@@ -4170,11 +4175,11 @@
         <v>322</v>
       </c>
       <c r="G64" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H64" s="2">
         <f t="shared" ref="H64:H81" si="3">D64*G64</f>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I64" t="s">
         <v>323</v>
@@ -4201,11 +4206,11 @@
         <v>325</v>
       </c>
       <c r="G65" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H65" s="2">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I65" t="s">
         <v>326</v>
@@ -4232,11 +4237,11 @@
         <v>328</v>
       </c>
       <c r="G66" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H66" s="2">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I66" t="s">
         <v>329</v>
@@ -4263,11 +4268,11 @@
         <v>331</v>
       </c>
       <c r="G67" s="2">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="H67" s="2">
         <f t="shared" si="3"/>
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="I67" t="s">
         <v>332</v>
@@ -4284,7 +4289,7 @@
         <v>357</v>
       </c>
       <c r="D68" s="1">
-        <f t="shared" ref="D68:D86" si="4">LEN(B68)-LEN(SUBSTITUTE(B68,",",""))+1</f>
+        <f t="shared" ref="D68:D85" si="4">LEN(B68)-LEN(SUBSTITUTE(B68,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="E68" t="s">
@@ -4294,11 +4299,11 @@
         <v>334</v>
       </c>
       <c r="G68" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H68" s="2">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I68" t="s">
         <v>335</v>
@@ -4325,11 +4330,11 @@
         <v>337</v>
       </c>
       <c r="G69" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H69" s="2">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I69" t="s">
         <v>338</v>
@@ -4356,11 +4361,11 @@
         <v>340</v>
       </c>
       <c r="G70" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H70" s="2">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I70" t="s">
         <v>341</v>
@@ -4387,11 +4392,11 @@
         <v>343</v>
       </c>
       <c r="G71" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H71" s="2">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I71" t="s">
         <v>344</v>
@@ -4418,11 +4423,11 @@
         <v>346</v>
       </c>
       <c r="G72" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H72" s="2">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I72" t="s">
         <v>347</v>
@@ -4449,11 +4454,11 @@
         <v>349</v>
       </c>
       <c r="G73" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H73" s="2">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I73" t="s">
         <v>350</v>
@@ -4480,11 +4485,11 @@
         <v>352</v>
       </c>
       <c r="G74" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H74" s="2">
         <f t="shared" si="3"/>
-        <v>0.70000000000000007</v>
+        <v>1.05</v>
       </c>
       <c r="I74" t="s">
         <v>353</v>
@@ -4511,11 +4516,11 @@
         <v>355</v>
       </c>
       <c r="G75" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H75" s="2">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I75" t="s">
         <v>356</v>
@@ -4542,11 +4547,11 @@
         <v>359</v>
       </c>
       <c r="G76" s="2">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="H76" s="2">
         <f t="shared" si="3"/>
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="I76" t="s">
         <v>360</v>
@@ -4573,11 +4578,11 @@
         <v>363</v>
       </c>
       <c r="G77" s="2">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="H77" s="2">
         <f t="shared" si="3"/>
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="I77" t="s">
         <v>364</v>
@@ -4604,11 +4609,11 @@
         <v>365</v>
       </c>
       <c r="G78" s="2">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="H78" s="2">
         <f t="shared" si="3"/>
-        <v>1.1200000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="I78" t="s">
         <v>366</v>
@@ -4635,11 +4640,11 @@
         <v>368</v>
       </c>
       <c r="G79" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H79" s="2">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I79" t="s">
         <v>369</v>
@@ -4660,20 +4665,20 @@
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="F80" t="s">
-        <v>427</v>
-      </c>
-      <c r="G80">
+        <v>424</v>
+      </c>
+      <c r="G80" s="3">
         <v>0.19</v>
       </c>
-      <c r="H80">
+      <c r="H80" s="3">
         <f t="shared" si="3"/>
         <v>0.19</v>
       </c>
       <c r="I80" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -4697,11 +4702,11 @@
         <v>371</v>
       </c>
       <c r="G81" s="2">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H81" s="2">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I81" t="s">
         <v>372</v>
@@ -4722,19 +4727,20 @@
         <v>7</v>
       </c>
       <c r="E82" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="F82" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="G82" s="2">
-        <v>0.61</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H82" s="2">
-        <v>4.2699999999999996</v>
+        <f>G82*D82</f>
+        <v>3.8500000000000005</v>
       </c>
       <c r="I82" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -4752,19 +4758,20 @@
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="F83" t="s">
         <v>168</v>
       </c>
       <c r="G83" s="2">
-        <v>0.9</v>
+        <v>0.81</v>
       </c>
       <c r="H83" s="2">
-        <v>0.9</v>
+        <f t="shared" ref="H83:H85" si="5">G83*D83</f>
+        <v>0.81</v>
       </c>
       <c r="I83" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -4782,19 +4789,20 @@
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F84" t="s">
         <v>171</v>
       </c>
       <c r="G84" s="2">
-        <v>1.1299999999999999</v>
+        <v>1.02</v>
       </c>
       <c r="H84" s="2">
-        <v>1.1299999999999999</v>
+        <f t="shared" si="5"/>
+        <v>1.02</v>
       </c>
       <c r="I84" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -4812,28 +4820,35 @@
         <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="F85" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G85" s="2">
-        <v>4.1100000000000003</v>
+        <v>5</v>
       </c>
       <c r="H85" s="2">
-        <v>4.1100000000000003</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="I85" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="D86" s="1"/>
       <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
+      <c r="H86" s="2">
+        <f>SUM(H2:H85)</f>
+        <v>39.67999999999995</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I74" r:id="rId1" xr:uid="{13D9BCB6-C6AC-4A50-A391-F4FDDFC241EC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Compared soldered passsive components to their measured value, and calculated the amplitude of the audio voltage signal at 42 and 100 percent system power
</commit_message>
<xml_diff>
--- a/Documents/BOM V2/Music_Visualizer_BOM_Digikey_Final_V2.xlsx
+++ b/Documents/BOM V2/Music_Visualizer_BOM_Digikey_Final_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\BOM V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C226EC-E192-40CC-A4B3-53C43B144991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D71EF32-9C5C-4745-8258-F0F7C3EAEE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19410" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Music_Visualizer" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="454">
   <si>
     <t>Comment</t>
   </si>
@@ -1329,6 +1329,72 @@
   </si>
   <si>
     <t>KAF15AR71H273JM</t>
+  </si>
+  <si>
+    <t>Issues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cap has a tolerance of 5%, max value should be 4.935, C13 = 5.535 and C14 = 4.995… </t>
+  </si>
+  <si>
+    <t>Not soldered yet</t>
+  </si>
+  <si>
+    <t>Max value should be 1.68, C19 = 2.376, C20=2.027</t>
+  </si>
+  <si>
+    <t>58.5k</t>
+  </si>
+  <si>
+    <t>R2 = 67.4k</t>
+  </si>
+  <si>
+    <t>R41 and R50 are fine</t>
+  </si>
+  <si>
+    <t>49.8k</t>
+  </si>
+  <si>
+    <t>R58 = 27.5k</t>
+  </si>
+  <si>
+    <t>R34 is fine</t>
+  </si>
+  <si>
+    <t>21.8k</t>
+  </si>
+  <si>
+    <t>10.53, more than 1 percent off…</t>
+  </si>
+  <si>
+    <t>Within 10 percent</t>
+  </si>
+  <si>
+    <t>about half within 20%, other half within 30%, 2 (C25 and C42) within 50%</t>
+  </si>
+  <si>
+    <t>both 26.3~nF</t>
+  </si>
+  <si>
+    <t>C43: 89UF, C44: 92uF</t>
+  </si>
+  <si>
+    <t>C58: 1.7uF</t>
+  </si>
+  <si>
+    <t>2.7nF</t>
+  </si>
+  <si>
+    <t>Check notes for this</t>
+  </si>
+  <si>
+    <t>within 5 percent</t>
+  </si>
+  <si>
+    <t>R39 = 35.6k</t>
+  </si>
+  <si>
+    <t>R48 is fine</t>
   </si>
 </sst>
 </file>
@@ -1821,11 +1887,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2183,28 +2252,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:K86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.77734375" customWidth="1"/>
-    <col min="3" max="3" width="81.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="90.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2232,8 +2301,11 @@
       <c r="I1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2263,8 +2335,9 @@
       <c r="I2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2294,8 +2367,9 @@
       <c r="I3" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2325,8 +2399,11 @@
       <c r="I4" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J4" s="5" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2356,8 +2433,11 @@
       <c r="I5" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J5" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2387,8 +2467,9 @@
       <c r="I6" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2418,8 +2499,11 @@
       <c r="I7" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J7" s="5" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -2449,8 +2533,11 @@
       <c r="I8" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J8" s="6" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2480,8 +2567,11 @@
       <c r="I9" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J9" s="6" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -2511,8 +2601,11 @@
       <c r="I10" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="4" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>421</v>
       </c>
@@ -2542,7 +2635,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -2572,8 +2665,11 @@
       <c r="I12" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J12" s="6" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2603,8 +2699,11 @@
       <c r="I13" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J13" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -2634,8 +2733,12 @@
       <c r="I14" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J14" s="4"/>
+      <c r="K14" s="5" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -2665,8 +2768,11 @@
       <c r="I15" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J15" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2696,8 +2802,11 @@
       <c r="I16" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J16" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2727,8 +2836,11 @@
       <c r="I17" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J17" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -2758,8 +2870,11 @@
       <c r="I18" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J18" s="6" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2789,8 +2904,11 @@
       <c r="I19" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J19" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -2820,8 +2938,11 @@
       <c r="I20" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J20" s="6" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -2851,8 +2972,11 @@
       <c r="I21" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J21" s="4" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -2882,8 +3006,11 @@
       <c r="I22" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J22" s="4" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -2914,7 +3041,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -2945,7 +3072,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -2975,8 +3102,11 @@
       <c r="I25" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J25" s="5" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -3006,8 +3136,11 @@
       <c r="I26" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J26" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -3037,8 +3170,11 @@
       <c r="I27" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J27" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -3068,8 +3204,9 @@
       <c r="I28" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -3099,8 +3236,11 @@
       <c r="I29" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J29" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -3130,8 +3270,11 @@
       <c r="I30" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J30" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -3161,8 +3304,11 @@
       <c r="I31" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J31" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>66</v>
       </c>
@@ -3192,8 +3338,9 @@
       <c r="I32" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>68</v>
       </c>
@@ -3223,8 +3370,11 @@
       <c r="I33" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J33" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>70</v>
       </c>
@@ -3254,8 +3404,11 @@
       <c r="I34" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J34" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -3285,8 +3438,14 @@
       <c r="I35" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J35" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -3316,8 +3475,11 @@
       <c r="I36" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J36" s="5" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>76</v>
       </c>
@@ -3347,8 +3509,11 @@
       <c r="I37" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J37" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>78</v>
       </c>
@@ -3378,8 +3543,9 @@
       <c r="I38" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>80</v>
       </c>
@@ -3409,8 +3575,9 @@
       <c r="I39" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>82</v>
       </c>
@@ -3440,8 +3607,9 @@
       <c r="I40" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>84</v>
       </c>
@@ -3471,8 +3639,11 @@
       <c r="I41" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J41" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -3502,8 +3673,11 @@
       <c r="I42" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J42" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -3533,8 +3707,11 @@
       <c r="I43" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J43" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>90</v>
       </c>
@@ -3564,8 +3741,9 @@
       <c r="I44" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J44" s="4"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>92</v>
       </c>
@@ -3595,8 +3773,9 @@
       <c r="I45" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J45" s="4"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>94</v>
       </c>
@@ -3626,8 +3805,11 @@
       <c r="I46" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J46" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>96</v>
       </c>
@@ -3657,8 +3839,11 @@
       <c r="I47" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J47" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>98</v>
       </c>
@@ -3688,8 +3873,11 @@
       <c r="I48" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J48" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>100</v>
       </c>
@@ -3719,8 +3907,14 @@
       <c r="I49" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J49" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>102</v>
       </c>
@@ -3750,8 +3944,9 @@
       <c r="I50" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J50" s="4"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>104</v>
       </c>
@@ -3781,8 +3976,11 @@
       <c r="I51" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J51" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>106</v>
       </c>
@@ -3812,8 +4010,14 @@
       <c r="I52" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J52" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>108</v>
       </c>
@@ -3843,8 +4047,9 @@
       <c r="I53" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J53" s="4"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>110</v>
       </c>
@@ -3874,8 +4079,11 @@
       <c r="I54" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J54" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>112</v>
       </c>
@@ -3905,8 +4113,9 @@
       <c r="I55" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J55" s="4"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>114</v>
       </c>
@@ -3936,8 +4145,11 @@
       <c r="I56" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J56" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>116</v>
       </c>
@@ -3967,8 +4179,11 @@
       <c r="I57" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J57" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>118</v>
       </c>
@@ -3998,8 +4213,9 @@
       <c r="I58" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J58" s="4"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>120</v>
       </c>
@@ -4029,8 +4245,11 @@
       <c r="I59" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J59" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>122</v>
       </c>
@@ -4060,8 +4279,9 @@
       <c r="I60" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J60" s="4"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>124</v>
       </c>
@@ -4091,8 +4311,11 @@
       <c r="I61" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J61" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>126</v>
       </c>
@@ -4122,8 +4345,11 @@
       <c r="I62" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J62" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>128</v>
       </c>
@@ -4153,8 +4379,11 @@
       <c r="I63" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J63" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>130</v>
       </c>
@@ -4184,8 +4413,9 @@
       <c r="I64" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J64" s="4"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>132</v>
       </c>
@@ -4215,8 +4445,11 @@
       <c r="I65" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J65" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>134</v>
       </c>
@@ -4246,8 +4479,11 @@
       <c r="I66" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J66" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>136</v>
       </c>
@@ -4277,8 +4513,11 @@
       <c r="I67" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J67" s="6" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>139</v>
       </c>
@@ -4308,8 +4547,11 @@
       <c r="I68" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J68" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>141</v>
       </c>
@@ -4339,8 +4581,11 @@
       <c r="I69" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J69" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>143</v>
       </c>
@@ -4370,8 +4615,11 @@
       <c r="I70" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J70" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>145</v>
       </c>
@@ -4401,8 +4649,9 @@
       <c r="I71" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J71" s="4"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>147</v>
       </c>
@@ -4432,8 +4681,11 @@
       <c r="I72" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J72" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>149</v>
       </c>
@@ -4463,8 +4715,11 @@
       <c r="I73" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J73" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>151</v>
       </c>
@@ -4494,8 +4749,9 @@
       <c r="I74" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J74" s="4"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>153</v>
       </c>
@@ -4525,8 +4781,11 @@
       <c r="I75" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J75" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>155</v>
       </c>
@@ -4556,8 +4815,9 @@
       <c r="I76" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J76" s="4"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>157</v>
       </c>
@@ -4587,8 +4847,9 @@
       <c r="I77" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J77" s="4"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>680</v>
       </c>
@@ -4618,8 +4879,9 @@
       <c r="I78" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J78" s="4"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>160</v>
       </c>
@@ -4649,8 +4911,9 @@
       <c r="I79" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J79" s="4"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>620</v>
       </c>
@@ -4680,8 +4943,9 @@
       <c r="I80" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J80" s="4"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>163</v>
       </c>
@@ -4711,8 +4975,11 @@
       <c r="I81" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="J81" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>165</v>
       </c>
@@ -4743,7 +5010,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>168</v>
       </c>
@@ -4774,7 +5041,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>171</v>
       </c>
@@ -4805,7 +5072,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>174</v>
       </c>
@@ -4836,7 +5103,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D86" s="1"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2">

</xml_diff>